<commit_message>
Update mosip-data with Guinea masterdata
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/individual_type.xlsx
+++ b/mosip_master/xlsx/individual_type.xlsx
@@ -1,33 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\materdata.xlxs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wuriguineecom-my.sharepoint.com/personal/iteli_bah_wuriguinee_com/Documents/Bureau/master-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D4D49612-BF1F-457A-9799-D13D57CFA2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C867F58F-AA4E-449A-960E-A7CA66962C56}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="9510" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
-  <si>
-    <t>lang_code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>code</t>
   </si>
@@ -35,73 +28,352 @@
     <t>name</t>
   </si>
   <si>
+    <t>lang_code</t>
+  </si>
+  <si>
     <t>is_active</t>
   </si>
   <si>
-    <t>eng</t>
+    <t>NFR</t>
+  </si>
+  <si>
+    <t>NON GUINEENNE</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
   <si>
     <t>FR</t>
   </si>
   <si>
-    <t>Foreigner</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>NFR</t>
-  </si>
-  <si>
-    <t>Non-Foreigner</t>
-  </si>
-  <si>
-    <t>fra</t>
-  </si>
-  <si>
-    <t>Étranger</t>
-  </si>
-  <si>
-    <t>Non-étranger</t>
-  </si>
-  <si>
-    <t>ara</t>
-  </si>
-  <si>
-    <t>أجنبي</t>
-  </si>
-  <si>
-    <t>غير أجنبي</t>
+    <t>GUINEENNE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <charset val="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -110,37 +382,203 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -156,7 +594,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -172,7 +610,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -184,7 +622,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -231,6 +669,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -266,6 +721,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -417,119 +889,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1"/>
+    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>